<commit_message>
Update C vs Python performance results.xlsx
</commit_message>
<xml_diff>
--- a/Results/C vs Python performance results.xlsx
+++ b/Results/C vs Python performance results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\C-vs-Python-performance-test\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\C-vs-Python-performance-test\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081EB92E-5CED-4872-9F33-4D1900FC1374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C9950C-64FE-42AA-B117-172F74A131FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -74,13 +72,13 @@
     <t>Testing Function 3 (bubble_sort)</t>
   </si>
   <si>
-    <t>Time [ms]</t>
-  </si>
-  <si>
     <t>Memory [KB]</t>
   </si>
   <si>
     <t>All test functions (custom average)</t>
+  </si>
+  <si>
+    <t>Time [s]</t>
   </si>
 </sst>
 </file>
@@ -265,9 +263,6 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,10 +282,13 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Izlaz" xfId="1" builtinId="21"/>
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -308,7 +306,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="hr-HR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -806,7 +804,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="hr-HR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1310,7 +1308,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="hr-HR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1808,7 +1806,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="hr-HR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2312,7 +2310,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="hr-HR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2818,7 +2816,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="hr-HR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3301,6 +3299,407 @@
           <a:ea typeface="+mn-ea"/>
           <a:cs typeface="+mn-cs"/>
         </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hr-HR"/>
+              <a:t>Memory</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="hr-HR" baseline="0"/>
+              <a:t> and time usage across all test functions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$S$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>List1!$T$11:$U$11</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Memory [KB]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time [s]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$T$12:$U$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>787.55599999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.150528033333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADD5-4287-A487-271EE495AF54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$S$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>List1!$T$11:$U$11</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Memory [KB]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time [s]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$T$13:$U$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>421.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4444668333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ADD5-4287-A487-271EE495AF54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="509915664"/>
+        <c:axId val="509914832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="509915664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509914832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="509914832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509915664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3553,6 +3952,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
   <cs:axisTitle>
@@ -6549,6 +6988,509 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -6779,6 +7721,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>229720</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>224118</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>128309</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B4823D6-F741-41D3-95CB-E6D79C1D43E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7047,8 +8025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7081,26 +8059,26 @@
       </c>
     </row>
     <row r="10" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="S10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="S10" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
     </row>
     <row r="11" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
@@ -7142,12 +8120,12 @@
       <c r="O11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S11" s="17"/>
-      <c r="T11" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="U11" s="19" t="s">
+      <c r="S11" s="16"/>
+      <c r="T11" s="18" t="s">
         <v>12</v>
+      </c>
+      <c r="U11" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="3:21" x14ac:dyDescent="0.25">
@@ -7192,16 +8170,16 @@
         <f>MEDIAN(D12:M12)</f>
         <v>1.367</v>
       </c>
-      <c r="S12" s="18" t="s">
+      <c r="S12" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="T12" s="20">
+      <c r="T12" s="19">
         <f xml:space="preserve"> AVERAGE(N13,O13,N22,O22,N31,O31)</f>
         <v>787.55599999999993</v>
       </c>
-      <c r="U12" s="21">
-        <f>AVERAGE(N12,O12,N21,O21,N30,O30)</f>
-        <v>44150.528033333336</v>
+      <c r="U12" s="20">
+        <f>AVERAGE(N12,O12,N21,O21,N30,O30)/1000</f>
+        <v>44.150528033333337</v>
       </c>
     </row>
     <row r="13" spans="3:21" x14ac:dyDescent="0.25">
@@ -7246,16 +8224,16 @@
         <f>MEDIAN(D13:M13)</f>
         <v>36.863999999999997</v>
       </c>
-      <c r="S13" s="18" t="s">
+      <c r="S13" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="T13" s="22">
+      <c r="T13" s="21">
         <f>AVERAGE(N15,O15,N24,O24,N33,O33)</f>
         <v>421.75</v>
       </c>
-      <c r="U13" s="23">
-        <f>AVERAGE(N14,O14,N23,O23,N32,O32)</f>
-        <v>1444.4668333333332</v>
+      <c r="U13" s="22">
+        <f>AVERAGE(N14,O14,N23,O23,N32,O32)/1000</f>
+        <v>1.4444668333333333</v>
       </c>
     </row>
     <row r="14" spans="3:21" x14ac:dyDescent="0.25">
@@ -7345,21 +8323,21 @@
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" s="7" t="s">
@@ -7575,21 +8553,21 @@
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C29" s="7" t="s">

</xml_diff>